<commit_message>
updated the excel data file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr date1904="false" showObjects="all" backupFile="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
@@ -12,17 +12,12 @@
     <sheet name="Countries" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Feuil3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="true" refMode="A1" iterate="false" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="17">
   <si>
     <t>Export (2014)</t>
   </si>
@@ -72,7 +67,7 @@
     <t>Total Export</t>
   </si>
   <si>
-    <t>total export</t>
+    <t>Created by LibXL trial version. Please buy the LibXL full version for removing this message.</t>
   </si>
 </sst>
 </file>
@@ -82,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -105,8 +100,12 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <color indexed="60"/>
+      <b/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,8 +136,13 @@
         <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="47"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -153,6 +157,7 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -179,7 +184,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -188,7 +193,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -196,7 +205,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -204,7 +213,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -219,6 +228,9 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -297,398 +309,666 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="C4 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.0242914979757"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.1093117408907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.080971659919"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="10.6032388663968"/>
+    <col min="1" max="1" width="47.348178137652" style="1" hidden="false" collapsed="false"/>
+    <col min="2" max="3" width="10.603238866397" style="1" hidden="false" collapsed="false"/>
+    <col min="4" max="4" width="14.141700404858" style="1" hidden="false" collapsed="false"/>
+    <col min="5" max="5" width="18.21052631579" style="1" hidden="false" collapsed="false"/>
+    <col min="6" max="1025" width="10.603238866397" style="1" hidden="false" collapsed="false"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11"/>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="11"/>
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11"/>
+      <c r="BJ1" s="11"/>
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11"/>
+      <c r="BN1" s="11"/>
+      <c r="BO1" s="11"/>
+      <c r="BP1" s="11"/>
+      <c r="BQ1" s="11"/>
+      <c r="BR1" s="11"/>
+      <c r="BS1" s="11"/>
+      <c r="BT1" s="11"/>
+      <c r="BU1" s="11"/>
+      <c r="BV1" s="11"/>
+      <c r="BW1" s="11"/>
+      <c r="BX1" s="11"/>
+      <c r="BY1" s="11"/>
+      <c r="BZ1" s="11"/>
+      <c r="CA1" s="11"/>
+      <c r="CB1" s="11"/>
+      <c r="CC1" s="11"/>
+      <c r="CD1" s="11"/>
+      <c r="CE1" s="11"/>
+      <c r="CF1" s="11"/>
+      <c r="CG1" s="11"/>
+      <c r="CH1" s="11"/>
+      <c r="CI1" s="11"/>
+      <c r="CJ1" s="11"/>
+      <c r="CK1" s="11"/>
+      <c r="CL1" s="11"/>
+      <c r="CM1" s="11"/>
+      <c r="CN1" s="11"/>
+      <c r="CO1" s="11"/>
+      <c r="CP1" s="11"/>
+      <c r="CQ1" s="11"/>
+      <c r="CR1" s="11"/>
+      <c r="CS1" s="11"/>
+      <c r="CT1" s="11"/>
+      <c r="CU1" s="11"/>
+      <c r="CV1" s="11"/>
+      <c r="CW1" s="11"/>
+      <c r="CX1" s="11"/>
+      <c r="CY1" s="11"/>
+      <c r="CZ1" s="11"/>
+      <c r="DA1" s="11"/>
+      <c r="DB1" s="11"/>
+      <c r="DC1" s="11"/>
+      <c r="DD1" s="11"/>
+      <c r="DE1" s="11"/>
+      <c r="DF1" s="11"/>
+      <c r="DG1" s="11"/>
+      <c r="DH1" s="11"/>
+      <c r="DI1" s="11"/>
+      <c r="DJ1" s="11"/>
+      <c r="DK1" s="11"/>
+      <c r="DL1" s="11"/>
+      <c r="DM1" s="11"/>
+      <c r="DN1" s="11"/>
+      <c r="DO1" s="11"/>
+      <c r="DP1" s="11"/>
+      <c r="DQ1" s="11"/>
+      <c r="DR1" s="11"/>
+      <c r="DS1" s="11"/>
+      <c r="DT1" s="11"/>
+      <c r="DU1" s="11"/>
+      <c r="DV1" s="11"/>
+      <c r="DW1" s="11"/>
+      <c r="DX1" s="11"/>
+      <c r="DY1" s="11"/>
+      <c r="DZ1" s="11"/>
+      <c r="EA1" s="11"/>
+      <c r="EB1" s="11"/>
+      <c r="EC1" s="11"/>
+      <c r="ED1" s="11"/>
+      <c r="EE1" s="11"/>
+      <c r="EF1" s="11"/>
+      <c r="EG1" s="11"/>
+      <c r="EH1" s="11"/>
+      <c r="EI1" s="11"/>
+      <c r="EJ1" s="11"/>
+      <c r="EK1" s="11"/>
+      <c r="EL1" s="11"/>
+      <c r="EM1" s="11"/>
+      <c r="EN1" s="11"/>
+      <c r="EO1" s="11"/>
+      <c r="EP1" s="11"/>
+      <c r="EQ1" s="11"/>
+      <c r="ER1" s="11"/>
+      <c r="ES1" s="11"/>
+      <c r="ET1" s="11"/>
+      <c r="EU1" s="11"/>
+      <c r="EV1" s="11"/>
+      <c r="EW1" s="11"/>
+      <c r="EX1" s="11"/>
+      <c r="EY1" s="11"/>
+      <c r="EZ1" s="11"/>
+      <c r="FA1" s="11"/>
+      <c r="FB1" s="11"/>
+      <c r="FC1" s="11"/>
+      <c r="FD1" s="11"/>
+      <c r="FE1" s="11"/>
+      <c r="FF1" s="11"/>
+      <c r="FG1" s="11"/>
+      <c r="FH1" s="11"/>
+      <c r="FI1" s="11"/>
+      <c r="FJ1" s="11"/>
+      <c r="FK1" s="11"/>
+      <c r="FL1" s="11"/>
+      <c r="FM1" s="11"/>
+      <c r="FN1" s="11"/>
+      <c r="FO1" s="11"/>
+      <c r="FP1" s="11"/>
+      <c r="FQ1" s="11"/>
+      <c r="FR1" s="11"/>
+      <c r="FS1" s="11"/>
+      <c r="FT1" s="11"/>
+      <c r="FU1" s="11"/>
+      <c r="FV1" s="11"/>
+      <c r="FW1" s="11"/>
+      <c r="FX1" s="11"/>
+      <c r="FY1" s="11"/>
+      <c r="FZ1" s="11"/>
+      <c r="GA1" s="11"/>
+      <c r="GB1" s="11"/>
+      <c r="GC1" s="11"/>
+      <c r="GD1" s="11"/>
+      <c r="GE1" s="11"/>
+      <c r="GF1" s="11"/>
+      <c r="GG1" s="11"/>
+      <c r="GH1" s="11"/>
+      <c r="GI1" s="11"/>
+      <c r="GJ1" s="11"/>
+      <c r="GK1" s="11"/>
+      <c r="GL1" s="11"/>
+      <c r="GM1" s="11"/>
+      <c r="GN1" s="11"/>
+      <c r="GO1" s="11"/>
+      <c r="GP1" s="11"/>
+      <c r="GQ1" s="11"/>
+      <c r="GR1" s="11"/>
+      <c r="GS1" s="11"/>
+      <c r="GT1" s="11"/>
+      <c r="GU1" s="11"/>
+      <c r="GV1" s="11"/>
+      <c r="GW1" s="11"/>
+      <c r="GX1" s="11"/>
+      <c r="GY1" s="11"/>
+      <c r="GZ1" s="11"/>
+      <c r="HA1" s="11"/>
+      <c r="HB1" s="11"/>
+      <c r="HC1" s="11"/>
+      <c r="HD1" s="11"/>
+      <c r="HE1" s="11"/>
+      <c r="HF1" s="11"/>
+      <c r="HG1" s="11"/>
+      <c r="HH1" s="11"/>
+      <c r="HI1" s="11"/>
+      <c r="HJ1" s="11"/>
+      <c r="HK1" s="11"/>
+      <c r="HL1" s="11"/>
+      <c r="HM1" s="11"/>
+      <c r="HN1" s="11"/>
+      <c r="HO1" s="11"/>
+      <c r="HP1" s="11"/>
+      <c r="HQ1" s="11"/>
+      <c r="HR1" s="11"/>
+      <c r="HS1" s="11"/>
+      <c r="HT1" s="11"/>
+      <c r="HU1" s="11"/>
+      <c r="HV1" s="11"/>
+      <c r="HW1" s="11"/>
+      <c r="HX1" s="11"/>
+      <c r="HY1" s="11"/>
+      <c r="HZ1" s="11"/>
+      <c r="IA1" s="11"/>
+      <c r="IB1" s="11"/>
+      <c r="IC1" s="11"/>
+      <c r="ID1" s="11"/>
+      <c r="IE1" s="11"/>
+      <c r="IF1" s="11"/>
+      <c r="IG1" s="11"/>
+      <c r="IH1" s="11"/>
+      <c r="II1" s="11"/>
+      <c r="IJ1" s="11"/>
+      <c r="IK1" s="11"/>
+      <c r="IL1" s="11"/>
+      <c r="IM1" s="11"/>
+      <c r="IN1" s="11"/>
+      <c r="IO1" s="11"/>
+      <c r="IP1" s="11"/>
+      <c r="IQ1" s="11"/>
+      <c r="IR1" s="11"/>
+      <c r="IS1" s="11"/>
+      <c r="IT1" s="11"/>
+      <c r="IU1" s="11"/>
+      <c r="IV1" s="11"/>
+    </row>
     <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="4" t="n">
         <v>17.7</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="n">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <v>15.2</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="3" t="n">
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="n">
         <v>20.9</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="4" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="3" t="n">
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="n">
         <v>0.976</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="n">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="n">
         <v>15.8</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="4" t="n">
         <v>1.43</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="4" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="6" t="n">
         <v>95.9</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="6" t="n">
         <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="5" t="n">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="6" t="n">
         <v>65.6</v>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" s="6" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="5" t="n">
+      <c r="C11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="6" t="n">
         <v>88.8</v>
       </c>
-      <c r="E11" s="5" t="n">
+      <c r="E11" s="6" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="5" t="n">
+      <c r="C12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="6" t="n">
         <v>3.39</v>
       </c>
-      <c r="E12" s="5" t="n">
+      <c r="E12" s="6" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="5" t="n">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="6" t="n">
         <v>158</v>
       </c>
-      <c r="E13" s="5" t="n">
+      <c r="E13" s="6" t="n">
         <v>58</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="D14" s="6" t="n">
         <v>16.2</v>
       </c>
-      <c r="E14" s="5" t="n">
+      <c r="E14" s="6" t="n">
         <v>69</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="8" t="n">
         <v>18.1</v>
       </c>
-      <c r="E15" s="7" t="n">
+      <c r="E15" s="8" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="7" t="n">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="8" t="n">
         <v>6.29</v>
       </c>
-      <c r="E16" s="7" t="n">
+      <c r="E16" s="8" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="7" t="n">
+      <c r="C17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="8" t="n">
         <v>98.9</v>
       </c>
-      <c r="E17" s="7" t="n">
+      <c r="E17" s="8" t="n">
         <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="7" t="n">
+      <c r="C18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="8" t="n">
         <v>0.0631</v>
       </c>
-      <c r="E18" s="7" t="n">
+      <c r="E18" s="8" t="n">
         <v>0.67</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="7" t="n">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="E19" s="7" t="n">
+      <c r="E19" s="8" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="7" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="7" t="n">
+      <c r="D20" s="8" t="n">
         <v>0.649</v>
       </c>
-      <c r="E20" s="7" t="n">
+      <c r="E20" s="8" t="n">
         <v>3</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+    </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8" t="s">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="9" t="n">
+      <c r="B24" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="D24" s="9" t="n">
+      <c r="D24" s="10" t="n">
         <v>225</v>
       </c>
-      <c r="E24" s="9" t="n">
+      <c r="E24" s="10" t="n">
         <v>165</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="9" t="n">
+      <c r="C25" s="10" t="n">
         <v>316</v>
       </c>
-      <c r="D25" s="9" t="n">
+      <c r="D25" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="E25" s="9" t="n">
+      <c r="E25" s="10" t="n">
         <v>9.39</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8"/>
-      <c r="B26" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="9" t="n">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="10" t="n">
         <v>271</v>
       </c>
-      <c r="D26" s="9" t="n">
+      <c r="D26" s="10" t="n">
         <v>23.6</v>
       </c>
-      <c r="E26" s="9" t="n">
+      <c r="E26" s="10" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="A15:A20"/>
     <mergeCell ref="A22:B23"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A1:IV1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <printOptions horizontalCentered="false" verticalCentered="false" headings="false" gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555" footer="0.51180555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <headerFooter differentOddEven="false" differentFirst="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
@@ -700,17 +980,277 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:J65536"/>
+  <dimension ref="A2:D1048576"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6032388663968"/>
+    <col min="1" max="1025" width="10.603238866397" style="0" hidden="false" collapsed="false"/>
   </cols>
   <sheetData>
+    <row r="1" ht="20" customHeight="true">
+      <c r="A1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11"/>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="11"/>
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11"/>
+      <c r="BJ1" s="11"/>
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11"/>
+      <c r="BN1" s="11"/>
+      <c r="BO1" s="11"/>
+      <c r="BP1" s="11"/>
+      <c r="BQ1" s="11"/>
+      <c r="BR1" s="11"/>
+      <c r="BS1" s="11"/>
+      <c r="BT1" s="11"/>
+      <c r="BU1" s="11"/>
+      <c r="BV1" s="11"/>
+      <c r="BW1" s="11"/>
+      <c r="BX1" s="11"/>
+      <c r="BY1" s="11"/>
+      <c r="BZ1" s="11"/>
+      <c r="CA1" s="11"/>
+      <c r="CB1" s="11"/>
+      <c r="CC1" s="11"/>
+      <c r="CD1" s="11"/>
+      <c r="CE1" s="11"/>
+      <c r="CF1" s="11"/>
+      <c r="CG1" s="11"/>
+      <c r="CH1" s="11"/>
+      <c r="CI1" s="11"/>
+      <c r="CJ1" s="11"/>
+      <c r="CK1" s="11"/>
+      <c r="CL1" s="11"/>
+      <c r="CM1" s="11"/>
+      <c r="CN1" s="11"/>
+      <c r="CO1" s="11"/>
+      <c r="CP1" s="11"/>
+      <c r="CQ1" s="11"/>
+      <c r="CR1" s="11"/>
+      <c r="CS1" s="11"/>
+      <c r="CT1" s="11"/>
+      <c r="CU1" s="11"/>
+      <c r="CV1" s="11"/>
+      <c r="CW1" s="11"/>
+      <c r="CX1" s="11"/>
+      <c r="CY1" s="11"/>
+      <c r="CZ1" s="11"/>
+      <c r="DA1" s="11"/>
+      <c r="DB1" s="11"/>
+      <c r="DC1" s="11"/>
+      <c r="DD1" s="11"/>
+      <c r="DE1" s="11"/>
+      <c r="DF1" s="11"/>
+      <c r="DG1" s="11"/>
+      <c r="DH1" s="11"/>
+      <c r="DI1" s="11"/>
+      <c r="DJ1" s="11"/>
+      <c r="DK1" s="11"/>
+      <c r="DL1" s="11"/>
+      <c r="DM1" s="11"/>
+      <c r="DN1" s="11"/>
+      <c r="DO1" s="11"/>
+      <c r="DP1" s="11"/>
+      <c r="DQ1" s="11"/>
+      <c r="DR1" s="11"/>
+      <c r="DS1" s="11"/>
+      <c r="DT1" s="11"/>
+      <c r="DU1" s="11"/>
+      <c r="DV1" s="11"/>
+      <c r="DW1" s="11"/>
+      <c r="DX1" s="11"/>
+      <c r="DY1" s="11"/>
+      <c r="DZ1" s="11"/>
+      <c r="EA1" s="11"/>
+      <c r="EB1" s="11"/>
+      <c r="EC1" s="11"/>
+      <c r="ED1" s="11"/>
+      <c r="EE1" s="11"/>
+      <c r="EF1" s="11"/>
+      <c r="EG1" s="11"/>
+      <c r="EH1" s="11"/>
+      <c r="EI1" s="11"/>
+      <c r="EJ1" s="11"/>
+      <c r="EK1" s="11"/>
+      <c r="EL1" s="11"/>
+      <c r="EM1" s="11"/>
+      <c r="EN1" s="11"/>
+      <c r="EO1" s="11"/>
+      <c r="EP1" s="11"/>
+      <c r="EQ1" s="11"/>
+      <c r="ER1" s="11"/>
+      <c r="ES1" s="11"/>
+      <c r="ET1" s="11"/>
+      <c r="EU1" s="11"/>
+      <c r="EV1" s="11"/>
+      <c r="EW1" s="11"/>
+      <c r="EX1" s="11"/>
+      <c r="EY1" s="11"/>
+      <c r="EZ1" s="11"/>
+      <c r="FA1" s="11"/>
+      <c r="FB1" s="11"/>
+      <c r="FC1" s="11"/>
+      <c r="FD1" s="11"/>
+      <c r="FE1" s="11"/>
+      <c r="FF1" s="11"/>
+      <c r="FG1" s="11"/>
+      <c r="FH1" s="11"/>
+      <c r="FI1" s="11"/>
+      <c r="FJ1" s="11"/>
+      <c r="FK1" s="11"/>
+      <c r="FL1" s="11"/>
+      <c r="FM1" s="11"/>
+      <c r="FN1" s="11"/>
+      <c r="FO1" s="11"/>
+      <c r="FP1" s="11"/>
+      <c r="FQ1" s="11"/>
+      <c r="FR1" s="11"/>
+      <c r="FS1" s="11"/>
+      <c r="FT1" s="11"/>
+      <c r="FU1" s="11"/>
+      <c r="FV1" s="11"/>
+      <c r="FW1" s="11"/>
+      <c r="FX1" s="11"/>
+      <c r="FY1" s="11"/>
+      <c r="FZ1" s="11"/>
+      <c r="GA1" s="11"/>
+      <c r="GB1" s="11"/>
+      <c r="GC1" s="11"/>
+      <c r="GD1" s="11"/>
+      <c r="GE1" s="11"/>
+      <c r="GF1" s="11"/>
+      <c r="GG1" s="11"/>
+      <c r="GH1" s="11"/>
+      <c r="GI1" s="11"/>
+      <c r="GJ1" s="11"/>
+      <c r="GK1" s="11"/>
+      <c r="GL1" s="11"/>
+      <c r="GM1" s="11"/>
+      <c r="GN1" s="11"/>
+      <c r="GO1" s="11"/>
+      <c r="GP1" s="11"/>
+      <c r="GQ1" s="11"/>
+      <c r="GR1" s="11"/>
+      <c r="GS1" s="11"/>
+      <c r="GT1" s="11"/>
+      <c r="GU1" s="11"/>
+      <c r="GV1" s="11"/>
+      <c r="GW1" s="11"/>
+      <c r="GX1" s="11"/>
+      <c r="GY1" s="11"/>
+      <c r="GZ1" s="11"/>
+      <c r="HA1" s="11"/>
+      <c r="HB1" s="11"/>
+      <c r="HC1" s="11"/>
+      <c r="HD1" s="11"/>
+      <c r="HE1" s="11"/>
+      <c r="HF1" s="11"/>
+      <c r="HG1" s="11"/>
+      <c r="HH1" s="11"/>
+      <c r="HI1" s="11"/>
+      <c r="HJ1" s="11"/>
+      <c r="HK1" s="11"/>
+      <c r="HL1" s="11"/>
+      <c r="HM1" s="11"/>
+      <c r="HN1" s="11"/>
+      <c r="HO1" s="11"/>
+      <c r="HP1" s="11"/>
+      <c r="HQ1" s="11"/>
+      <c r="HR1" s="11"/>
+      <c r="HS1" s="11"/>
+      <c r="HT1" s="11"/>
+      <c r="HU1" s="11"/>
+      <c r="HV1" s="11"/>
+      <c r="HW1" s="11"/>
+      <c r="HX1" s="11"/>
+      <c r="HY1" s="11"/>
+      <c r="HZ1" s="11"/>
+      <c r="IA1" s="11"/>
+      <c r="IB1" s="11"/>
+      <c r="IC1" s="11"/>
+      <c r="ID1" s="11"/>
+      <c r="IE1" s="11"/>
+      <c r="IF1" s="11"/>
+      <c r="IG1" s="11"/>
+      <c r="IH1" s="11"/>
+      <c r="II1" s="11"/>
+      <c r="IJ1" s="11"/>
+      <c r="IK1" s="11"/>
+      <c r="IL1" s="11"/>
+      <c r="IM1" s="11"/>
+      <c r="IN1" s="11"/>
+      <c r="IO1" s="11"/>
+      <c r="IP1" s="11"/>
+      <c r="IQ1" s="11"/>
+      <c r="IR1" s="11"/>
+      <c r="IS1" s="11"/>
+      <c r="IT1" s="11"/>
+      <c r="IU1" s="11"/>
+      <c r="IV1" s="11"/>
+    </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>6</v>
@@ -726,6 +1266,15 @@
       <c r="A3" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="B3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -741,30 +1290,24 @@
         <v>384</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I21" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J23" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
+    <row r="6">
+      <c r="A6">
+        <v>3.2999999999999998</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:IV1"/>
+  </mergeCells>
+  <printOptions horizontalCentered="false" verticalCentered="false" headings="false" gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555" footer="0.51180555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <headerFooter differentOddEven="false" differentFirst="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
@@ -779,18 +1322,282 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6032388663968"/>
+    <col min="1" max="1025" width="10.603238866397" style="0" hidden="false" collapsed="false"/>
   </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <sheetData>
+    <row r="1" ht="20" customHeight="true">
+      <c r="A1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11"/>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="11"/>
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11"/>
+      <c r="BJ1" s="11"/>
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11"/>
+      <c r="BN1" s="11"/>
+      <c r="BO1" s="11"/>
+      <c r="BP1" s="11"/>
+      <c r="BQ1" s="11"/>
+      <c r="BR1" s="11"/>
+      <c r="BS1" s="11"/>
+      <c r="BT1" s="11"/>
+      <c r="BU1" s="11"/>
+      <c r="BV1" s="11"/>
+      <c r="BW1" s="11"/>
+      <c r="BX1" s="11"/>
+      <c r="BY1" s="11"/>
+      <c r="BZ1" s="11"/>
+      <c r="CA1" s="11"/>
+      <c r="CB1" s="11"/>
+      <c r="CC1" s="11"/>
+      <c r="CD1" s="11"/>
+      <c r="CE1" s="11"/>
+      <c r="CF1" s="11"/>
+      <c r="CG1" s="11"/>
+      <c r="CH1" s="11"/>
+      <c r="CI1" s="11"/>
+      <c r="CJ1" s="11"/>
+      <c r="CK1" s="11"/>
+      <c r="CL1" s="11"/>
+      <c r="CM1" s="11"/>
+      <c r="CN1" s="11"/>
+      <c r="CO1" s="11"/>
+      <c r="CP1" s="11"/>
+      <c r="CQ1" s="11"/>
+      <c r="CR1" s="11"/>
+      <c r="CS1" s="11"/>
+      <c r="CT1" s="11"/>
+      <c r="CU1" s="11"/>
+      <c r="CV1" s="11"/>
+      <c r="CW1" s="11"/>
+      <c r="CX1" s="11"/>
+      <c r="CY1" s="11"/>
+      <c r="CZ1" s="11"/>
+      <c r="DA1" s="11"/>
+      <c r="DB1" s="11"/>
+      <c r="DC1" s="11"/>
+      <c r="DD1" s="11"/>
+      <c r="DE1" s="11"/>
+      <c r="DF1" s="11"/>
+      <c r="DG1" s="11"/>
+      <c r="DH1" s="11"/>
+      <c r="DI1" s="11"/>
+      <c r="DJ1" s="11"/>
+      <c r="DK1" s="11"/>
+      <c r="DL1" s="11"/>
+      <c r="DM1" s="11"/>
+      <c r="DN1" s="11"/>
+      <c r="DO1" s="11"/>
+      <c r="DP1" s="11"/>
+      <c r="DQ1" s="11"/>
+      <c r="DR1" s="11"/>
+      <c r="DS1" s="11"/>
+      <c r="DT1" s="11"/>
+      <c r="DU1" s="11"/>
+      <c r="DV1" s="11"/>
+      <c r="DW1" s="11"/>
+      <c r="DX1" s="11"/>
+      <c r="DY1" s="11"/>
+      <c r="DZ1" s="11"/>
+      <c r="EA1" s="11"/>
+      <c r="EB1" s="11"/>
+      <c r="EC1" s="11"/>
+      <c r="ED1" s="11"/>
+      <c r="EE1" s="11"/>
+      <c r="EF1" s="11"/>
+      <c r="EG1" s="11"/>
+      <c r="EH1" s="11"/>
+      <c r="EI1" s="11"/>
+      <c r="EJ1" s="11"/>
+      <c r="EK1" s="11"/>
+      <c r="EL1" s="11"/>
+      <c r="EM1" s="11"/>
+      <c r="EN1" s="11"/>
+      <c r="EO1" s="11"/>
+      <c r="EP1" s="11"/>
+      <c r="EQ1" s="11"/>
+      <c r="ER1" s="11"/>
+      <c r="ES1" s="11"/>
+      <c r="ET1" s="11"/>
+      <c r="EU1" s="11"/>
+      <c r="EV1" s="11"/>
+      <c r="EW1" s="11"/>
+      <c r="EX1" s="11"/>
+      <c r="EY1" s="11"/>
+      <c r="EZ1" s="11"/>
+      <c r="FA1" s="11"/>
+      <c r="FB1" s="11"/>
+      <c r="FC1" s="11"/>
+      <c r="FD1" s="11"/>
+      <c r="FE1" s="11"/>
+      <c r="FF1" s="11"/>
+      <c r="FG1" s="11"/>
+      <c r="FH1" s="11"/>
+      <c r="FI1" s="11"/>
+      <c r="FJ1" s="11"/>
+      <c r="FK1" s="11"/>
+      <c r="FL1" s="11"/>
+      <c r="FM1" s="11"/>
+      <c r="FN1" s="11"/>
+      <c r="FO1" s="11"/>
+      <c r="FP1" s="11"/>
+      <c r="FQ1" s="11"/>
+      <c r="FR1" s="11"/>
+      <c r="FS1" s="11"/>
+      <c r="FT1" s="11"/>
+      <c r="FU1" s="11"/>
+      <c r="FV1" s="11"/>
+      <c r="FW1" s="11"/>
+      <c r="FX1" s="11"/>
+      <c r="FY1" s="11"/>
+      <c r="FZ1" s="11"/>
+      <c r="GA1" s="11"/>
+      <c r="GB1" s="11"/>
+      <c r="GC1" s="11"/>
+      <c r="GD1" s="11"/>
+      <c r="GE1" s="11"/>
+      <c r="GF1" s="11"/>
+      <c r="GG1" s="11"/>
+      <c r="GH1" s="11"/>
+      <c r="GI1" s="11"/>
+      <c r="GJ1" s="11"/>
+      <c r="GK1" s="11"/>
+      <c r="GL1" s="11"/>
+      <c r="GM1" s="11"/>
+      <c r="GN1" s="11"/>
+      <c r="GO1" s="11"/>
+      <c r="GP1" s="11"/>
+      <c r="GQ1" s="11"/>
+      <c r="GR1" s="11"/>
+      <c r="GS1" s="11"/>
+      <c r="GT1" s="11"/>
+      <c r="GU1" s="11"/>
+      <c r="GV1" s="11"/>
+      <c r="GW1" s="11"/>
+      <c r="GX1" s="11"/>
+      <c r="GY1" s="11"/>
+      <c r="GZ1" s="11"/>
+      <c r="HA1" s="11"/>
+      <c r="HB1" s="11"/>
+      <c r="HC1" s="11"/>
+      <c r="HD1" s="11"/>
+      <c r="HE1" s="11"/>
+      <c r="HF1" s="11"/>
+      <c r="HG1" s="11"/>
+      <c r="HH1" s="11"/>
+      <c r="HI1" s="11"/>
+      <c r="HJ1" s="11"/>
+      <c r="HK1" s="11"/>
+      <c r="HL1" s="11"/>
+      <c r="HM1" s="11"/>
+      <c r="HN1" s="11"/>
+      <c r="HO1" s="11"/>
+      <c r="HP1" s="11"/>
+      <c r="HQ1" s="11"/>
+      <c r="HR1" s="11"/>
+      <c r="HS1" s="11"/>
+      <c r="HT1" s="11"/>
+      <c r="HU1" s="11"/>
+      <c r="HV1" s="11"/>
+      <c r="HW1" s="11"/>
+      <c r="HX1" s="11"/>
+      <c r="HY1" s="11"/>
+      <c r="HZ1" s="11"/>
+      <c r="IA1" s="11"/>
+      <c r="IB1" s="11"/>
+      <c r="IC1" s="11"/>
+      <c r="ID1" s="11"/>
+      <c r="IE1" s="11"/>
+      <c r="IF1" s="11"/>
+      <c r="IG1" s="11"/>
+      <c r="IH1" s="11"/>
+      <c r="II1" s="11"/>
+      <c r="IJ1" s="11"/>
+      <c r="IK1" s="11"/>
+      <c r="IL1" s="11"/>
+      <c r="IM1" s="11"/>
+      <c r="IN1" s="11"/>
+      <c r="IO1" s="11"/>
+      <c r="IP1" s="11"/>
+      <c r="IQ1" s="11"/>
+      <c r="IR1" s="11"/>
+      <c r="IS1" s="11"/>
+      <c r="IT1" s="11"/>
+      <c r="IU1" s="11"/>
+      <c r="IV1" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:IV1"/>
+  </mergeCells>
+  <printOptions horizontalCentered="false" verticalCentered="false" headings="false" gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555" footer="0.51180555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <headerFooter differentOddEven="false" differentFirst="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>

</xml_diff>

<commit_message>
finalised the functions to read Excel data file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Markets" sheetId="1" state="visible" r:id="rId2"/>
@@ -312,16 +312,16 @@
   </sheetPr>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.7732793522267"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -729,7 +729,7 @@
   </sheetPr>
   <dimension ref="A2:D21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added values for countries
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr date1904="false" showObjects="all" backupFile="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Markets" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Countries" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Feuil3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr fullCalcOnLoad="true" refMode="A1" iterate="false" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -328,17 +333,17 @@
   </sheetPr>
   <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="48.631578947368" style="1" hidden="false" collapsed="false"/>
-    <col min="2" max="3" width="10.603238866397" style="1" hidden="false" collapsed="false"/>
-    <col min="4" max="4" width="14.141700404858" style="1" hidden="false" collapsed="false"/>
-    <col min="5" max="5" width="18.53036437247" style="1" hidden="false" collapsed="false"/>
-    <col min="6" max="1025" width="10.603238866397" style="1" hidden="false" collapsed="false"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.1417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -982,10 +987,10 @@
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="A24:A26"/>
   </mergeCells>
-  <printOptions horizontalCentered="false" verticalCentered="false" headings="false" gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555" footer="0.51180555555555"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false">
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
@@ -997,15 +1002,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IV24"/>
+  <dimension ref="A1:IV21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="10.603238866397" style="0" hidden="false" collapsed="false"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1286,14 +1292,14 @@
       <c r="A3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" s="0" t="n">
+        <v>17419000000000</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>2</v>
+        <v>1601799527772</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>3</v>
+        <v>2171020370398</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,13 +1307,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>14430</v>
+        <v>2341900000000</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>440</v>
+        <v>564422936007</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>384</v>
+        <v>419381937183</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1315,13 +1321,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>330</v>
+        <v>2851524000000</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>580864446023</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>3</v>
+        <v>433976892027</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1329,13 +1335,13 @@
         <v>18</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>2</v>
+        <v>-1.36</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>3</v>
+        <v>-1.56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1343,13 +1349,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1</v>
+        <v>1.451</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>2</v>
+        <v>2.249</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>3</v>
+        <v>1.143</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1357,13 +1363,16 @@
         <v>20</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1</v>
+        <f aca="false">B3-B4+B5</f>
+        <v>17928624000000</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>2</v>
+        <f aca="false">C3-C4+C5</f>
+        <v>1618241037788</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>3</v>
+        <f aca="false">D3-D4+D5</f>
+        <v>2185615325242</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1376,10 +1385,10 @@
   <mergeCells count="1">
     <mergeCell ref="A1:IV1"/>
   </mergeCells>
-  <printOptions horizontalCentered="false" verticalCentered="false" headings="false" gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555" footer="0.51180555555555"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false">
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
@@ -1399,7 +1408,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="10.603238866397" style="0" hidden="false" collapsed="false"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1666,10 +1675,10 @@
   <mergeCells count="1">
     <mergeCell ref="A1:IV1"/>
   </mergeCells>
-  <printOptions horizontalCentered="false" verticalCentered="false" headings="false" gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555" footer="0.51180555555555"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false">
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>

</xml_diff>

<commit_message>
Fixed problem with billions
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="20">
   <si>
     <t>Created by LibXL trial version. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Elasticity exports</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
 </sst>
 </file>
@@ -339,10 +336,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="49.4898785425101"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -1005,12 +1002,12 @@
   <dimension ref="A1:IV21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -1293,13 +1290,13 @@
         <v>16</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>17419000000000</v>
+        <v>17419</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>1601799527772</v>
+        <v>1602</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>2171020370398</v>
+        <v>2171.020370398</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1307,13 +1304,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>2341900000000</v>
+        <v>2341.9</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>564422936007</v>
+        <v>564.422936007</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>419381937183</v>
+        <v>419.381937183</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1321,13 +1318,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>2851524000000</v>
+        <v>2851.524</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>580864446023</v>
+        <v>580.864446023</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>433976892027</v>
+        <v>433.976892027</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,23 +1353,6 @@
       </c>
       <c r="D7" s="0" t="n">
         <v>1.143</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <f aca="false">B3-B4+B5</f>
-        <v>17928624000000</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <f aca="false">C3-C4+C5</f>
-        <v>1618241037788</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <f aca="false">D3-D4+D5</f>
-        <v>2185615325242</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>